<commit_message>
Update namespaces and fix typo in test spreadsheets
</commit_message>
<xml_diff>
--- a/src/integration-test/resources/multiDataModelImport.xlsx
+++ b/src/integration-test/resources/multiDataModelImport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ollie/code/metadata-catalogue/mc-plugins/mc-plugin-excel/src/integration-test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjl/code/maurodatamapper-plugins/mdm-plugin-excel/src/integration-test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4738E4-1980-AF43-B5B9-917F1387A7F0}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048777D0-3738-FC4C-A5E1-DD07E6020476}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20280" xr2:uid="{C2FC2BFD-8D7E-AA4E-A82C-4DBAFEC0EBFC}"/>
   </bookViews>
   <sheets>
     <sheet name="DataModels" sheetId="1" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>yesno</t>
   </si>
   <si>
-    <t>an eumeration</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -519,7 +516,10 @@
     <t>COMPLEX</t>
   </si>
   <si>
-    <t>ox.softeng.metadatacatalogue.plugins.xsd</t>
+    <t>an enumeration</t>
+  </si>
+  <si>
+    <t>uk.ac.ox.softeng.maurodatamapper.plugins.xsd</t>
   </si>
 </sst>
 </file>
@@ -938,6 +938,43 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -988,43 +1025,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1343,7 +1343,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,53 +1355,53 @@
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="26" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="47" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="63" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:10" s="35" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="52" t="s">
+      <c r="C1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="I1" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="33" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="23" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62" t="s">
-        <v>75</v>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="34" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="33" thickTop="1" x14ac:dyDescent="0.2">
@@ -1424,25 +1424,25 @@
         <v>22</v>
       </c>
       <c r="G3" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>20</v>
@@ -1451,23 +1451,23 @@
         <v>21</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="12"/>
@@ -1479,7 +1479,7 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +1515,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1543,10 +1543,10 @@
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -1555,20 +1555,20 @@
       <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="48" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1579,13 +1579,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="36"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1595,7 +1595,7 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1638,7 +1638,7 @@
         <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
@@ -1678,111 +1678,111 @@
         <v>27</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="50">
         <v>0</v>
       </c>
-      <c r="E8" s="37">
+      <c r="E8" s="50">
         <v>-1</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="H8" s="50"/>
+      <c r="I8" t="s">
         <v>38</v>
       </c>
-      <c r="H8" s="37"/>
-      <c r="I8" t="s">
+      <c r="J8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="1" t="s">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" t="s">
+      <c r="J9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>44</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>45</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="37"/>
+      <c r="A11" s="50"/>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="37"/>
+      <c r="A12" s="50"/>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1793,13 +1793,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1811,7 +1811,7 @@
         <v>32</v>
       </c>
       <c r="K14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1819,16 +1819,16 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
         <v>58</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>60</v>
-      </c>
-      <c r="G15" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1836,10 +1836,10 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" t="s">
-        <v>63</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1883,7 +1883,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="G9" sqref="G9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1911,10 +1911,10 @@
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="46" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -1923,20 +1923,20 @@
       <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="48" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1947,13 +1947,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="36"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="49"/>
     </row>
     <row r="3" spans="1:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1963,7 +1963,7 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1971,22 +1971,22 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
         <v>69</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>70</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>71</v>
-      </c>
-      <c r="G4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -2029,7 +2029,7 @@
         <v>31</v>
       </c>
       <c r="K6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L6" t="s">
         <v>25</v>
@@ -2069,53 +2069,53 @@
         <v>27</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="40">
-        <v>1</v>
-      </c>
-      <c r="E9" s="40">
+      <c r="D9" s="53">
+        <v>1</v>
+      </c>
+      <c r="E9" s="53">
         <v>-1</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="37" t="s">
+      <c r="G9" s="50" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="50"/>
+      <c r="I9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="37"/>
-      <c r="I9" t="s">
+      <c r="J9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="37"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" t="s">
+      <c r="J10" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2123,27 +2123,27 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>59</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>60</v>
-      </c>
-      <c r="G11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -2154,13 +2154,13 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
         <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2172,18 +2172,18 @@
         <v>32</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -2250,44 +2250,44 @@
       <c r="B1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="45" t="s">
+      <c r="C1" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="L1" s="45" t="s">
+      <c r="K1" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="L1" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="45" t="s">
+      <c r="M1" s="58" t="s">
         <v>158</v>
       </c>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="58" t="s">
         <v>157</v>
+      </c>
+      <c r="O1" s="58" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="29" customFormat="1" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2297,19 +2297,19 @@
       <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
     </row>
     <row r="3" spans="1:15" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
@@ -2330,11 +2330,11 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -2351,13 +2351,13 @@
     </row>
     <row r="5" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
@@ -2366,16 +2366,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="11"/>
       <c r="K5" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -2384,13 +2384,13 @@
     </row>
     <row r="6" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
@@ -2399,16 +2399,16 @@
         <v>1</v>
       </c>
       <c r="F6" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
       <c r="J6" s="27"/>
       <c r="K6" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
@@ -2417,10 +2417,10 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="9">
@@ -2430,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="9"/>
@@ -2444,11 +2444,11 @@
     </row>
     <row r="8" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="26">
         <v>1</v>
@@ -2469,28 +2469,28 @@
     </row>
     <row r="9" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>153</v>
-      </c>
       <c r="G9" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="11"/>
@@ -2502,13 +2502,13 @@
     </row>
     <row r="10" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" s="26">
         <v>1</v>
@@ -2517,7 +2517,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G10" s="28"/>
       <c r="H10" s="26"/>
@@ -2531,10 +2531,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="9">
@@ -2544,11 +2544,11 @@
         <v>1</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
@@ -2560,28 +2560,28 @@
     </row>
     <row r="12" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26">
+        <v>1</v>
+      </c>
+      <c r="F12" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="26">
-        <v>1</v>
-      </c>
-      <c r="E12" s="26">
-        <v>1</v>
-      </c>
-      <c r="F12" s="26" t="s">
-        <v>147</v>
-      </c>
       <c r="G12" s="28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="26"/>
       <c r="J12" s="27"/>
@@ -2593,10 +2593,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="9">
@@ -2606,11 +2606,11 @@
         <v>1</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="11"/>
@@ -2622,13 +2622,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D14" s="26">
         <v>1</v>
@@ -2637,7 +2637,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G14" s="28"/>
       <c r="H14" s="26"/>
@@ -2651,11 +2651,11 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
@@ -2672,10 +2672,10 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="28"/>
       <c r="D16" s="26">
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16" s="28"/>
       <c r="H16" s="26"/>
@@ -2693,7 +2693,7 @@
       <c r="J16" s="27"/>
       <c r="K16" s="26"/>
       <c r="L16" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M16" s="26"/>
       <c r="N16" s="26"/>
@@ -2701,10 +2701,10 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="9">
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="9"/>
@@ -2722,7 +2722,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="9"/>
       <c r="L17" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -2730,11 +2730,11 @@
     </row>
     <row r="18" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="26"/>
@@ -2746,20 +2746,20 @@
       <c r="K18" s="26"/>
       <c r="L18" s="26"/>
       <c r="M18" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N18" s="26"/>
       <c r="O18" s="26"/>
     </row>
     <row r="19" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19" s="9">
         <v>1</v>
@@ -2768,16 +2768,16 @@
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="J19" s="11"/>
       <c r="K19" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -2786,13 +2786,13 @@
     </row>
     <row r="20" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D20" s="26">
         <v>1</v>
@@ -2801,16 +2801,16 @@
         <v>1</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
       <c r="J20" s="27"/>
       <c r="K20" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L20" s="26"/>
       <c r="M20" s="26"/>
@@ -2819,10 +2819,10 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>124</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="9">
@@ -2832,10 +2832,10 @@
         <v>1</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
@@ -2848,10 +2848,10 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="26">
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G22" s="28"/>
       <c r="H22" s="26"/>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="10"/>
@@ -2894,10 +2894,10 @@
     </row>
     <row r="24" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="26">
@@ -2907,13 +2907,13 @@
         <v>1</v>
       </c>
       <c r="F24" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="28" t="s">
-        <v>82</v>
-      </c>
       <c r="H24" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="26"/>
       <c r="J24" s="27"/>
@@ -2925,10 +2925,10 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="9">
@@ -2938,10 +2938,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
@@ -2954,10 +2954,10 @@
     </row>
     <row r="26" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="26">
@@ -2967,16 +2967,16 @@
         <v>1</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="27"/>
       <c r="K26" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L26" s="26"/>
       <c r="M26" s="26"/>
@@ -2985,10 +2985,10 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="9">
@@ -2998,14 +2998,14 @@
         <v>1</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="11"/>
       <c r="K27" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
@@ -3014,10 +3014,10 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="26">
@@ -3027,14 +3027,14 @@
         <v>-1</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G28" s="28"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="27"/>
       <c r="K28" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L28" s="26"/>
       <c r="M28" s="26"/>
@@ -3043,10 +3043,10 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="9">
@@ -3056,14 +3056,14 @@
         <v>-1</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G29" s="10"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="11"/>
       <c r="K29" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
@@ -3072,10 +3072,10 @@
     </row>
     <row r="30" spans="1:15" ht="64" x14ac:dyDescent="0.2">
       <c r="A30" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="26">
@@ -3085,13 +3085,13 @@
         <v>1</v>
       </c>
       <c r="F30" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="G30" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="28" t="s">
-        <v>82</v>
-      </c>
       <c r="H30" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
@@ -3103,7 +3103,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="10"/>
@@ -3122,13 +3122,13 @@
     </row>
     <row r="32" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="26">
         <v>1</v>
@@ -3140,7 +3140,7 @@
         <v>27</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H32" s="26"/>
       <c r="I32" s="26"/>
@@ -3149,173 +3149,173 @@
       <c r="L32" s="26"/>
       <c r="M32" s="26"/>
       <c r="N32" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="O32" s="26"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="43" t="s">
+      <c r="A33" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="D33" s="42">
-        <v>1</v>
-      </c>
-      <c r="E33" s="42">
-        <v>1</v>
-      </c>
-      <c r="F33" s="42" t="s">
+      <c r="C33" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="G33" s="43" t="s">
+      <c r="D33" s="55">
+        <v>1</v>
+      </c>
+      <c r="E33" s="55">
+        <v>1</v>
+      </c>
+      <c r="F33" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="H33" s="42"/>
+      <c r="G33" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="H33" s="55"/>
       <c r="I33" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="K33" s="42"/>
-      <c r="L33" s="42"/>
-      <c r="M33" s="42"/>
-      <c r="N33" s="42"/>
-      <c r="O33" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="K33" s="55"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="55"/>
+      <c r="N33" s="55"/>
+      <c r="O33" s="56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="55"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="J34" s="27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A34" s="42"/>
-      <c r="B34" s="42"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="J34" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="55"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
+      <c r="A35" s="55"/>
+      <c r="B35" s="55"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42"/>
-      <c r="O35" s="42"/>
+        <v>91</v>
+      </c>
+      <c r="K35" s="55"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="55"/>
+      <c r="N35" s="55"/>
+      <c r="O35" s="55"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36" s="41" t="s">
+      <c r="A36" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="D36" s="41">
+      <c r="D36" s="54">
         <v>0</v>
       </c>
-      <c r="E36" s="41">
-        <v>1</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36" s="44"/>
-      <c r="H36" s="41"/>
+      <c r="E36" s="54">
+        <v>1</v>
+      </c>
+      <c r="F36" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="57"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41"/>
+        <v>87</v>
+      </c>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="54"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="41"/>
+      <c r="A37" s="54"/>
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="41"/>
+        <v>85</v>
+      </c>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
-      <c r="C38" s="41"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="41"/>
+      <c r="A38" s="54"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
       <c r="I38" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J38" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-    </row>
-    <row r="39" spans="1:15" ht="64" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+    </row>
+    <row r="39" spans="1:15" ht="68" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D39" s="9">
         <v>1</v>
@@ -3324,13 +3324,13 @@
         <v>-1</v>
       </c>
       <c r="F39" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>82</v>
-      </c>
       <c r="H39" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I39" s="9"/>
       <c r="J39" s="11"/>
@@ -3340,15 +3340,15 @@
       <c r="N39" s="9"/>
       <c r="O39" s="9"/>
     </row>
-    <row r="40" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A40" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="26">
         <v>1</v>
@@ -3357,10 +3357,10 @@
         <v>1</v>
       </c>
       <c r="F40" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H40" s="26"/>
       <c r="I40" s="26"/>

</xml_diff>